<commit_message>
add robust test and unit time/cost assessment
</commit_message>
<xml_diff>
--- a/master_data.xlsx
+++ b/master_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leizhang/Desktop/thesis_xixi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Desktop/Thesis_xixi/ Masterthesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9A3B7F-DF07-7C4D-8DC4-AE2E623A1526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C252E4F-18E6-9D4B-A1F0-02EFCDE66F6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="520" windowWidth="28800" windowHeight="16080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16080" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kpi_tech" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="constraints" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -233,8 +233,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="184" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -764,16 +764,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -789,18 +789,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -843,62 +831,74 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="184" fontId="6" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1193,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+    <sheetView zoomScale="115" workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
@@ -1218,34 +1218,34 @@
   <sheetData>
     <row r="2" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="66" t="s">
+      <c r="C3" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="66" t="s">
+      <c r="E3" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="66" t="s">
+      <c r="H3" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="66" t="s">
+      <c r="I3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="66" t="s">
+      <c r="J3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="67" t="s">
+      <c r="K3" s="58" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="6" t="s">
@@ -1268,46 +1268,46 @@
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="59">
+      <c r="C4" s="50">
         <v>0.9821428571428571</v>
       </c>
-      <c r="D4" s="59">
+      <c r="D4" s="50">
         <v>0.97340425531914898</v>
       </c>
-      <c r="E4" s="59">
+      <c r="E4" s="50">
         <v>-2.6595744680851019E-2</v>
       </c>
-      <c r="F4" s="59">
-        <v>0</v>
-      </c>
-      <c r="G4" s="59">
+      <c r="F4" s="50">
+        <v>0</v>
+      </c>
+      <c r="G4" s="50">
         <v>-2.6595744680851019E-2</v>
       </c>
-      <c r="H4" s="59">
-        <v>0</v>
-      </c>
-      <c r="I4" s="59">
+      <c r="H4" s="50">
+        <v>0</v>
+      </c>
+      <c r="I4" s="50">
         <v>-0.33333333333333337</v>
       </c>
-      <c r="J4" s="59">
+      <c r="J4" s="50">
         <v>7.6923076923076872E-2</v>
       </c>
-      <c r="K4" s="63">
-        <v>0</v>
-      </c>
-      <c r="L4" s="60">
-        <v>0</v>
-      </c>
-      <c r="M4" s="60">
-        <v>0</v>
-      </c>
-      <c r="N4" s="60">
-        <v>0</v>
-      </c>
-      <c r="O4" s="60">
-        <v>0</v>
-      </c>
-      <c r="P4" s="62">
+      <c r="K4" s="54">
+        <v>0</v>
+      </c>
+      <c r="L4" s="51">
+        <v>0</v>
+      </c>
+      <c r="M4" s="51">
+        <v>0</v>
+      </c>
+      <c r="N4" s="51">
+        <v>0</v>
+      </c>
+      <c r="O4" s="51">
+        <v>0</v>
+      </c>
+      <c r="P4" s="53">
         <v>0</v>
       </c>
     </row>
@@ -1315,46 +1315,46 @@
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="50">
         <v>0.91803278688524592</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="50">
         <v>0.89074803149606296</v>
       </c>
-      <c r="E5" s="59">
+      <c r="E5" s="50">
         <v>-0.10925196850393704</v>
       </c>
-      <c r="F5" s="59">
+      <c r="F5" s="50">
         <v>-0.4</v>
       </c>
-      <c r="G5" s="59">
+      <c r="G5" s="50">
         <v>-0.10853478046373954</v>
       </c>
-      <c r="H5" s="59">
-        <v>0</v>
-      </c>
-      <c r="I5" s="59">
-        <v>0</v>
-      </c>
-      <c r="J5" s="59">
-        <v>0</v>
-      </c>
-      <c r="K5" s="63">
+      <c r="H5" s="50">
+        <v>0</v>
+      </c>
+      <c r="I5" s="50">
+        <v>0</v>
+      </c>
+      <c r="J5" s="50">
+        <v>0</v>
+      </c>
+      <c r="K5" s="54">
         <v>-0.19999999999999996</v>
       </c>
-      <c r="L5" s="59">
-        <v>0</v>
-      </c>
-      <c r="M5" s="59">
-        <v>0</v>
-      </c>
-      <c r="N5" s="59">
-        <v>0</v>
-      </c>
-      <c r="O5" s="59">
-        <v>0</v>
-      </c>
-      <c r="P5" s="63">
+      <c r="L5" s="50">
+        <v>0</v>
+      </c>
+      <c r="M5" s="50">
+        <v>0</v>
+      </c>
+      <c r="N5" s="50">
+        <v>0</v>
+      </c>
+      <c r="O5" s="50">
+        <v>0</v>
+      </c>
+      <c r="P5" s="54">
         <v>0</v>
       </c>
     </row>
@@ -1362,46 +1362,46 @@
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="59">
+      <c r="C6" s="50">
         <v>0.92561983471074383</v>
       </c>
-      <c r="D6" s="59">
+      <c r="D6" s="50">
         <v>0.91321897073662972</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="50">
         <v>-8.678102926337028E-2</v>
       </c>
-      <c r="F6" s="59">
+      <c r="F6" s="50">
         <v>-0.5</v>
       </c>
-      <c r="G6" s="59">
+      <c r="G6" s="50">
         <v>-8.5526315789473673E-2</v>
       </c>
-      <c r="H6" s="59">
-        <v>0</v>
-      </c>
-      <c r="I6" s="59">
-        <v>0</v>
-      </c>
-      <c r="J6" s="59">
-        <v>0</v>
-      </c>
-      <c r="K6" s="63">
-        <v>0</v>
-      </c>
-      <c r="L6" s="59">
-        <v>0</v>
-      </c>
-      <c r="M6" s="59">
-        <v>0</v>
-      </c>
-      <c r="N6" s="59">
-        <v>0</v>
-      </c>
-      <c r="O6" s="59">
-        <v>0</v>
-      </c>
-      <c r="P6" s="63">
+      <c r="H6" s="50">
+        <v>0</v>
+      </c>
+      <c r="I6" s="50">
+        <v>0</v>
+      </c>
+      <c r="J6" s="50">
+        <v>0</v>
+      </c>
+      <c r="K6" s="54">
+        <v>0</v>
+      </c>
+      <c r="L6" s="50">
+        <v>0</v>
+      </c>
+      <c r="M6" s="50">
+        <v>0</v>
+      </c>
+      <c r="N6" s="50">
+        <v>0</v>
+      </c>
+      <c r="O6" s="50">
+        <v>0</v>
+      </c>
+      <c r="P6" s="54">
         <v>0</v>
       </c>
     </row>
@@ -1409,46 +1409,46 @@
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="59">
-        <v>1</v>
-      </c>
-      <c r="D7" s="59">
-        <v>1</v>
-      </c>
-      <c r="E7" s="59">
-        <v>0</v>
-      </c>
-      <c r="F7" s="59">
-        <v>0</v>
-      </c>
-      <c r="G7" s="59">
-        <v>0</v>
-      </c>
-      <c r="H7" s="59">
-        <v>0</v>
-      </c>
-      <c r="I7" s="59">
+      <c r="C7" s="50">
+        <v>1</v>
+      </c>
+      <c r="D7" s="50">
+        <v>1</v>
+      </c>
+      <c r="E7" s="50">
+        <v>0</v>
+      </c>
+      <c r="F7" s="50">
+        <v>0</v>
+      </c>
+      <c r="G7" s="50">
+        <v>0</v>
+      </c>
+      <c r="H7" s="50">
+        <v>0</v>
+      </c>
+      <c r="I7" s="50">
         <v>-0.33333333333333337</v>
       </c>
-      <c r="J7" s="59">
+      <c r="J7" s="50">
         <v>7.6923076923076872E-2</v>
       </c>
-      <c r="K7" s="63">
-        <v>0</v>
-      </c>
-      <c r="L7" s="59">
-        <v>0</v>
-      </c>
-      <c r="M7" s="59">
-        <v>0</v>
-      </c>
-      <c r="N7" s="59">
-        <v>0</v>
-      </c>
-      <c r="O7" s="59">
-        <v>0</v>
-      </c>
-      <c r="P7" s="63">
+      <c r="K7" s="54">
+        <v>0</v>
+      </c>
+      <c r="L7" s="50">
+        <v>0</v>
+      </c>
+      <c r="M7" s="50">
+        <v>0</v>
+      </c>
+      <c r="N7" s="50">
+        <v>0</v>
+      </c>
+      <c r="O7" s="50">
+        <v>0</v>
+      </c>
+      <c r="P7" s="54">
         <v>0</v>
       </c>
     </row>
@@ -1456,46 +1456,46 @@
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="59">
+      <c r="C8" s="50">
         <v>0.9145299145299145</v>
       </c>
-      <c r="D8" s="59">
+      <c r="D8" s="50">
         <v>0.87064676616915426</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="50">
         <v>-0.12935323383084574</v>
       </c>
-      <c r="F8" s="59">
+      <c r="F8" s="50">
         <v>-0.33333333333333337</v>
       </c>
-      <c r="G8" s="59">
+      <c r="G8" s="50">
         <v>-0.12843578210894557</v>
       </c>
-      <c r="H8" s="59">
-        <v>0</v>
-      </c>
-      <c r="I8" s="59">
+      <c r="H8" s="50">
+        <v>0</v>
+      </c>
+      <c r="I8" s="50">
         <v>-0.1</v>
       </c>
-      <c r="J8" s="59">
+      <c r="J8" s="50">
         <v>7.1428571428571397E-2</v>
       </c>
-      <c r="K8" s="63">
-        <v>0</v>
-      </c>
-      <c r="L8" s="59">
-        <v>0</v>
-      </c>
-      <c r="M8" s="59">
-        <v>0</v>
-      </c>
-      <c r="N8" s="59">
-        <v>0</v>
-      </c>
-      <c r="O8" s="59">
-        <v>0</v>
-      </c>
-      <c r="P8" s="63">
+      <c r="K8" s="54">
+        <v>0</v>
+      </c>
+      <c r="L8" s="50">
+        <v>0</v>
+      </c>
+      <c r="M8" s="50">
+        <v>0</v>
+      </c>
+      <c r="N8" s="50">
+        <v>0</v>
+      </c>
+      <c r="O8" s="50">
+        <v>0</v>
+      </c>
+      <c r="P8" s="54">
         <v>0</v>
       </c>
     </row>
@@ -1503,46 +1503,46 @@
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="59">
-        <v>1</v>
-      </c>
-      <c r="D9" s="59">
-        <v>1</v>
-      </c>
-      <c r="E9" s="59">
-        <v>0</v>
-      </c>
-      <c r="F9" s="59">
-        <v>0</v>
-      </c>
-      <c r="G9" s="59">
-        <v>0</v>
-      </c>
-      <c r="H9" s="59">
-        <v>0</v>
-      </c>
-      <c r="I9" s="59">
-        <v>0</v>
-      </c>
-      <c r="J9" s="59">
-        <v>0</v>
-      </c>
-      <c r="K9" s="63">
-        <v>0</v>
-      </c>
-      <c r="L9" s="59">
+      <c r="C9" s="50">
+        <v>1</v>
+      </c>
+      <c r="D9" s="50">
+        <v>1</v>
+      </c>
+      <c r="E9" s="50">
+        <v>0</v>
+      </c>
+      <c r="F9" s="50">
+        <v>0</v>
+      </c>
+      <c r="G9" s="50">
+        <v>0</v>
+      </c>
+      <c r="H9" s="50">
+        <v>0</v>
+      </c>
+      <c r="I9" s="50">
+        <v>0</v>
+      </c>
+      <c r="J9" s="50">
+        <v>0</v>
+      </c>
+      <c r="K9" s="54">
+        <v>0</v>
+      </c>
+      <c r="L9" s="50">
         <v>-1</v>
       </c>
-      <c r="M9" s="59">
-        <v>0</v>
-      </c>
-      <c r="N9" s="59">
+      <c r="M9" s="50">
+        <v>0</v>
+      </c>
+      <c r="N9" s="50">
         <v>-1</v>
       </c>
-      <c r="O9" s="59">
-        <v>0</v>
-      </c>
-      <c r="P9" s="63">
+      <c r="O9" s="50">
+        <v>0</v>
+      </c>
+      <c r="P9" s="54">
         <v>0</v>
       </c>
     </row>
@@ -1550,46 +1550,46 @@
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="59">
+      <c r="C10" s="50">
         <v>0.95726495726495731</v>
       </c>
-      <c r="D10" s="59">
+      <c r="D10" s="50">
         <v>0.94467640918580376</v>
       </c>
-      <c r="E10" s="59">
+      <c r="E10" s="50">
         <v>-5.5323590814196244E-2</v>
       </c>
-      <c r="F10" s="59">
+      <c r="F10" s="50">
         <v>-0.5</v>
       </c>
-      <c r="G10" s="59">
+      <c r="G10" s="50">
         <v>-5.392670157068058E-2</v>
       </c>
-      <c r="H10" s="59">
-        <v>0</v>
-      </c>
-      <c r="I10" s="59">
-        <v>0</v>
-      </c>
-      <c r="J10" s="59">
-        <v>0</v>
-      </c>
-      <c r="K10" s="63">
-        <v>0</v>
-      </c>
-      <c r="L10" s="59">
-        <v>0</v>
-      </c>
-      <c r="M10" s="59">
-        <v>0</v>
-      </c>
-      <c r="N10" s="59">
-        <v>0</v>
-      </c>
-      <c r="O10" s="59">
-        <v>0</v>
-      </c>
-      <c r="P10" s="63">
+      <c r="H10" s="50">
+        <v>0</v>
+      </c>
+      <c r="I10" s="50">
+        <v>0</v>
+      </c>
+      <c r="J10" s="50">
+        <v>0</v>
+      </c>
+      <c r="K10" s="54">
+        <v>0</v>
+      </c>
+      <c r="L10" s="50">
+        <v>0</v>
+      </c>
+      <c r="M10" s="50">
+        <v>0</v>
+      </c>
+      <c r="N10" s="50">
+        <v>0</v>
+      </c>
+      <c r="O10" s="50">
+        <v>0</v>
+      </c>
+      <c r="P10" s="54">
         <v>0</v>
       </c>
     </row>
@@ -1597,46 +1597,46 @@
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="59">
-        <v>1</v>
-      </c>
-      <c r="D11" s="59">
-        <v>1</v>
-      </c>
-      <c r="E11" s="59">
-        <v>0</v>
-      </c>
-      <c r="F11" s="59">
-        <v>0</v>
-      </c>
-      <c r="G11" s="59">
-        <v>0</v>
-      </c>
-      <c r="H11" s="59">
-        <v>0</v>
-      </c>
-      <c r="I11" s="59">
-        <v>0</v>
-      </c>
-      <c r="J11" s="59">
-        <v>0</v>
-      </c>
-      <c r="K11" s="63">
-        <v>0</v>
-      </c>
-      <c r="L11" s="59">
+      <c r="C11" s="50">
+        <v>1</v>
+      </c>
+      <c r="D11" s="50">
+        <v>1</v>
+      </c>
+      <c r="E11" s="50">
+        <v>0</v>
+      </c>
+      <c r="F11" s="50">
+        <v>0</v>
+      </c>
+      <c r="G11" s="50">
+        <v>0</v>
+      </c>
+      <c r="H11" s="50">
+        <v>0</v>
+      </c>
+      <c r="I11" s="50">
+        <v>0</v>
+      </c>
+      <c r="J11" s="50">
+        <v>0</v>
+      </c>
+      <c r="K11" s="54">
+        <v>0</v>
+      </c>
+      <c r="L11" s="50">
         <v>-0.66666666666666674</v>
       </c>
-      <c r="M11" s="59">
-        <v>0</v>
-      </c>
-      <c r="N11" s="59">
-        <v>0</v>
-      </c>
-      <c r="O11" s="59">
+      <c r="M11" s="50">
+        <v>0</v>
+      </c>
+      <c r="N11" s="50">
+        <v>0</v>
+      </c>
+      <c r="O11" s="50">
         <v>-0.22727272727272729</v>
       </c>
-      <c r="P11" s="63">
+      <c r="P11" s="54">
         <v>0</v>
       </c>
     </row>
@@ -1644,46 +1644,46 @@
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="59">
+      <c r="C12" s="50">
         <v>0.94117647058823528</v>
       </c>
-      <c r="D12" s="59">
+      <c r="D12" s="50">
         <v>0.92346938775510201</v>
       </c>
-      <c r="E12" s="59">
+      <c r="E12" s="50">
         <v>-7.6530612244897989E-2</v>
       </c>
-      <c r="F12" s="59">
-        <v>0</v>
-      </c>
-      <c r="G12" s="59">
+      <c r="F12" s="50">
+        <v>0</v>
+      </c>
+      <c r="G12" s="50">
         <v>-7.6647930505876372E-2</v>
       </c>
-      <c r="H12" s="59">
-        <v>0</v>
-      </c>
-      <c r="I12" s="59">
-        <v>0</v>
-      </c>
-      <c r="J12" s="59">
-        <v>0</v>
-      </c>
-      <c r="K12" s="63">
-        <v>0</v>
-      </c>
-      <c r="L12" s="59">
-        <v>0</v>
-      </c>
-      <c r="M12" s="59">
-        <v>0</v>
-      </c>
-      <c r="N12" s="59">
-        <v>0</v>
-      </c>
-      <c r="O12" s="59">
-        <v>0</v>
-      </c>
-      <c r="P12" s="63">
+      <c r="H12" s="50">
+        <v>0</v>
+      </c>
+      <c r="I12" s="50">
+        <v>0</v>
+      </c>
+      <c r="J12" s="50">
+        <v>0</v>
+      </c>
+      <c r="K12" s="54">
+        <v>0</v>
+      </c>
+      <c r="L12" s="50">
+        <v>0</v>
+      </c>
+      <c r="M12" s="50">
+        <v>0</v>
+      </c>
+      <c r="N12" s="50">
+        <v>0</v>
+      </c>
+      <c r="O12" s="50">
+        <v>0</v>
+      </c>
+      <c r="P12" s="54">
         <v>0</v>
       </c>
     </row>
@@ -1691,46 +1691,46 @@
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="59">
-        <v>1</v>
-      </c>
-      <c r="D13" s="59">
-        <v>1</v>
-      </c>
-      <c r="E13" s="59">
-        <v>0</v>
-      </c>
-      <c r="F13" s="59">
-        <v>0</v>
-      </c>
-      <c r="G13" s="59">
-        <v>0</v>
-      </c>
-      <c r="H13" s="59">
-        <v>0</v>
-      </c>
-      <c r="I13" s="59">
-        <v>0</v>
-      </c>
-      <c r="J13" s="59">
-        <v>0</v>
-      </c>
-      <c r="K13" s="63">
-        <v>0</v>
-      </c>
-      <c r="L13" s="59">
-        <v>0</v>
-      </c>
-      <c r="M13" s="59">
-        <v>0</v>
-      </c>
-      <c r="N13" s="59">
-        <v>0</v>
-      </c>
-      <c r="O13" s="59">
-        <v>0</v>
-      </c>
-      <c r="P13" s="63">
+      <c r="C13" s="50">
+        <v>1</v>
+      </c>
+      <c r="D13" s="50">
+        <v>1</v>
+      </c>
+      <c r="E13" s="50">
+        <v>0</v>
+      </c>
+      <c r="F13" s="50">
+        <v>0</v>
+      </c>
+      <c r="G13" s="50">
+        <v>0</v>
+      </c>
+      <c r="H13" s="50">
+        <v>0</v>
+      </c>
+      <c r="I13" s="50">
+        <v>0</v>
+      </c>
+      <c r="J13" s="50">
+        <v>0</v>
+      </c>
+      <c r="K13" s="54">
+        <v>0</v>
+      </c>
+      <c r="L13" s="50">
+        <v>0</v>
+      </c>
+      <c r="M13" s="50">
+        <v>0</v>
+      </c>
+      <c r="N13" s="50">
+        <v>0</v>
+      </c>
+      <c r="O13" s="50">
+        <v>0</v>
+      </c>
+      <c r="P13" s="54">
         <v>-0.66666666666666674</v>
       </c>
     </row>
@@ -1738,46 +1738,46 @@
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="59">
+      <c r="C14" s="50">
         <v>0.95726495726495731</v>
       </c>
-      <c r="D14" s="59">
+      <c r="D14" s="50">
         <v>0.93782383419689119</v>
       </c>
-      <c r="E14" s="59">
+      <c r="E14" s="50">
         <v>-6.2176165803108807E-2</v>
       </c>
-      <c r="F14" s="59">
+      <c r="F14" s="50">
         <v>-0.625</v>
       </c>
-      <c r="G14" s="59">
+      <c r="G14" s="50">
         <v>-5.9833506763787736E-2</v>
       </c>
-      <c r="H14" s="59">
-        <v>0</v>
-      </c>
-      <c r="I14" s="59">
-        <v>0</v>
-      </c>
-      <c r="J14" s="59">
-        <v>0</v>
-      </c>
-      <c r="K14" s="63">
+      <c r="H14" s="50">
+        <v>0</v>
+      </c>
+      <c r="I14" s="50">
+        <v>0</v>
+      </c>
+      <c r="J14" s="50">
+        <v>0</v>
+      </c>
+      <c r="K14" s="54">
         <v>-0.19999999999999996</v>
       </c>
-      <c r="L14" s="59">
-        <v>0</v>
-      </c>
-      <c r="M14" s="59">
-        <v>0</v>
-      </c>
-      <c r="N14" s="59">
-        <v>0</v>
-      </c>
-      <c r="O14" s="59">
-        <v>0</v>
-      </c>
-      <c r="P14" s="63">
+      <c r="L14" s="50">
+        <v>0</v>
+      </c>
+      <c r="M14" s="50">
+        <v>0</v>
+      </c>
+      <c r="N14" s="50">
+        <v>0</v>
+      </c>
+      <c r="O14" s="50">
+        <v>0</v>
+      </c>
+      <c r="P14" s="54">
         <v>-0.66666666666666674</v>
       </c>
     </row>
@@ -1785,46 +1785,46 @@
       <c r="B15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="61">
-        <v>1</v>
-      </c>
-      <c r="D15" s="61">
-        <v>1</v>
-      </c>
-      <c r="E15" s="61">
-        <v>0</v>
-      </c>
-      <c r="F15" s="61">
-        <v>0</v>
-      </c>
-      <c r="G15" s="61">
-        <v>0</v>
-      </c>
-      <c r="H15" s="61">
-        <v>0</v>
-      </c>
-      <c r="I15" s="61">
-        <v>0</v>
-      </c>
-      <c r="J15" s="61">
-        <v>0</v>
-      </c>
-      <c r="K15" s="64">
-        <v>0</v>
-      </c>
-      <c r="L15" s="61">
-        <v>0</v>
-      </c>
-      <c r="M15" s="61">
-        <v>0</v>
-      </c>
-      <c r="N15" s="61">
-        <v>0</v>
-      </c>
-      <c r="O15" s="61">
-        <v>0</v>
-      </c>
-      <c r="P15" s="64">
+      <c r="C15" s="52">
+        <v>1</v>
+      </c>
+      <c r="D15" s="52">
+        <v>1</v>
+      </c>
+      <c r="E15" s="52">
+        <v>0</v>
+      </c>
+      <c r="F15" s="52">
+        <v>0</v>
+      </c>
+      <c r="G15" s="52">
+        <v>0</v>
+      </c>
+      <c r="H15" s="52">
+        <v>0</v>
+      </c>
+      <c r="I15" s="52">
+        <v>0</v>
+      </c>
+      <c r="J15" s="52">
+        <v>0</v>
+      </c>
+      <c r="K15" s="55">
+        <v>0</v>
+      </c>
+      <c r="L15" s="52">
+        <v>0</v>
+      </c>
+      <c r="M15" s="52">
+        <v>0</v>
+      </c>
+      <c r="N15" s="52">
+        <v>0</v>
+      </c>
+      <c r="O15" s="52">
+        <v>0</v>
+      </c>
+      <c r="P15" s="55">
         <v>-0.58830409356725144</v>
       </c>
     </row>
@@ -2400,8 +2400,8 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="15" t="s">
         <v>25</v>
       </c>
@@ -2440,8 +2440,8 @@
       </c>
     </row>
     <row r="4" spans="2:15" ht="64" x14ac:dyDescent="0.2">
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="16" t="s">
         <v>17</v>
       </c>
@@ -2480,462 +2480,462 @@
       </c>
     </row>
     <row r="5" spans="2:15" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="48">
+      <c r="B5" s="44">
         <v>1</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="43">
         <v>1.05</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="43">
         <v>1.0666666666666667</v>
       </c>
-      <c r="F5" s="47">
-        <v>1</v>
-      </c>
-      <c r="G5" s="47">
-        <v>1</v>
-      </c>
-      <c r="H5" s="47">
-        <v>1</v>
-      </c>
-      <c r="I5" s="47">
+      <c r="F5" s="43">
+        <v>1</v>
+      </c>
+      <c r="G5" s="43">
+        <v>1</v>
+      </c>
+      <c r="H5" s="43">
+        <v>1</v>
+      </c>
+      <c r="I5" s="43">
         <v>1.05</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J5" s="43">
         <v>1.0333333333333334</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="43">
         <v>1.0333333333333334</v>
       </c>
-      <c r="L5" s="47">
-        <v>1</v>
-      </c>
-      <c r="M5" s="47">
+      <c r="L5" s="43">
+        <v>1</v>
+      </c>
+      <c r="M5" s="43">
         <v>1.0666666666666667</v>
       </c>
-      <c r="N5" s="47">
+      <c r="N5" s="43">
         <v>1.0666666666666667</v>
       </c>
-      <c r="O5" s="47">
+      <c r="O5" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="48">
+      <c r="B6" s="44">
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="43">
         <v>0.9</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="43">
         <v>0.96666666666666667</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="43">
         <v>0.9</v>
       </c>
-      <c r="G6" s="47">
+      <c r="G6" s="43">
         <v>0.95</v>
       </c>
-      <c r="H6" s="47">
+      <c r="H6" s="43">
         <v>0.9</v>
       </c>
-      <c r="I6" s="47">
+      <c r="I6" s="43">
         <v>0.95</v>
       </c>
-      <c r="J6" s="47">
-        <v>1</v>
-      </c>
-      <c r="K6" s="47">
-        <v>1</v>
-      </c>
-      <c r="L6" s="47">
+      <c r="J6" s="43">
+        <v>1</v>
+      </c>
+      <c r="K6" s="43">
+        <v>1</v>
+      </c>
+      <c r="L6" s="43">
         <v>0.95</v>
       </c>
-      <c r="M6" s="47">
-        <v>1</v>
-      </c>
-      <c r="N6" s="47">
+      <c r="M6" s="43">
+        <v>1</v>
+      </c>
+      <c r="N6" s="43">
         <v>0.9</v>
       </c>
-      <c r="O6" s="47">
+      <c r="O6" s="43">
         <v>0.95</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="48">
+      <c r="B7" s="44">
         <v>3</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="43">
         <v>1.0333333333333334</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F7" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G7" s="47">
+      <c r="G7" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H7" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J7" s="47">
+      <c r="J7" s="43">
         <v>1.0333333333333334</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="43">
         <v>1.0333333333333334</v>
       </c>
-      <c r="L7" s="47">
+      <c r="L7" s="43">
         <v>1.05</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="43">
         <v>1.0666666666666667</v>
       </c>
-      <c r="N7" s="47">
+      <c r="N7" s="43">
         <v>1.0666666666666667</v>
       </c>
-      <c r="O7" s="47">
+      <c r="O7" s="43">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="48">
+      <c r="B8" s="44">
         <v>4</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="43">
         <v>1.05</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="43">
         <v>0.96666666666666667</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="43">
         <v>0.95</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="43">
         <v>0.95</v>
       </c>
-      <c r="I8" s="47">
-        <v>1</v>
-      </c>
-      <c r="J8" s="47">
-        <v>1</v>
-      </c>
-      <c r="K8" s="47">
-        <v>1</v>
-      </c>
-      <c r="L8" s="47">
+      <c r="I8" s="43">
+        <v>1</v>
+      </c>
+      <c r="J8" s="43">
+        <v>1</v>
+      </c>
+      <c r="K8" s="43">
+        <v>1</v>
+      </c>
+      <c r="L8" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M8" s="47">
+      <c r="M8" s="43">
         <v>1.0666666666666667</v>
       </c>
-      <c r="N8" s="47">
+      <c r="N8" s="43">
         <v>1.0333333333333334</v>
       </c>
-      <c r="O8" s="47">
+      <c r="O8" s="43">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="48">
+      <c r="B9" s="44">
         <v>5</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="47">
-        <v>1</v>
-      </c>
-      <c r="E9" s="47">
-        <v>1</v>
-      </c>
-      <c r="F9" s="47">
-        <v>1</v>
-      </c>
-      <c r="G9" s="47">
-        <v>1</v>
-      </c>
-      <c r="H9" s="47">
-        <v>1</v>
-      </c>
-      <c r="I9" s="47">
+      <c r="D9" s="43">
+        <v>1</v>
+      </c>
+      <c r="E9" s="43">
+        <v>1</v>
+      </c>
+      <c r="F9" s="43">
+        <v>1</v>
+      </c>
+      <c r="G9" s="43">
+        <v>1</v>
+      </c>
+      <c r="H9" s="43">
+        <v>1</v>
+      </c>
+      <c r="I9" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J9" s="47">
+      <c r="J9" s="43">
         <v>1.0666666666666667</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K9" s="43">
         <v>1.0333333333333334</v>
       </c>
-      <c r="L9" s="47">
-        <v>1</v>
-      </c>
-      <c r="M9" s="47">
+      <c r="L9" s="43">
+        <v>1</v>
+      </c>
+      <c r="M9" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N9" s="47">
+      <c r="N9" s="43">
         <v>1.0333333333333334</v>
       </c>
-      <c r="O9" s="47">
+      <c r="O9" s="43">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="48">
+      <c r="B10" s="44">
         <v>6</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="43">
         <v>1.05</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="43">
         <v>1.05</v>
       </c>
-      <c r="H10" s="47">
+      <c r="H10" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I10" s="47">
+      <c r="I10" s="43">
         <v>1.05</v>
       </c>
-      <c r="J10" s="47">
+      <c r="J10" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K10" s="47">
+      <c r="K10" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L10" s="47">
+      <c r="L10" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M10" s="47">
+      <c r="M10" s="43">
         <v>1.0666666666666667</v>
       </c>
-      <c r="N10" s="47">
+      <c r="N10" s="43">
         <v>1.0666666666666667</v>
       </c>
-      <c r="O10" s="47">
+      <c r="O10" s="43">
         <v>1.05</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="48">
+      <c r="B11" s="44">
         <v>7</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="43">
         <v>1.05</v>
       </c>
-      <c r="E11" s="47">
-        <v>1</v>
-      </c>
-      <c r="F11" s="47">
+      <c r="E11" s="43">
+        <v>1</v>
+      </c>
+      <c r="F11" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G11" s="47">
+      <c r="G11" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H11" s="47">
+      <c r="H11" s="43">
         <v>1.05</v>
       </c>
-      <c r="I11" s="47">
-        <v>1</v>
-      </c>
-      <c r="J11" s="47">
-        <v>1</v>
-      </c>
-      <c r="K11" s="47">
-        <v>1</v>
-      </c>
-      <c r="L11" s="47">
+      <c r="I11" s="43">
+        <v>1</v>
+      </c>
+      <c r="J11" s="43">
+        <v>1</v>
+      </c>
+      <c r="K11" s="43">
+        <v>1</v>
+      </c>
+      <c r="L11" s="43">
         <v>1.05</v>
       </c>
-      <c r="M11" s="47">
+      <c r="M11" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N11" s="47">
+      <c r="N11" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O11" s="47">
+      <c r="O11" s="43">
         <v>1.05</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="49"/>
-      <c r="C12" s="50" t="s">
+      <c r="B12" s="45"/>
+      <c r="C12" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="47">
         <f>D5*D6*D7*D8*D9*D10*D11</f>
         <v>1.2033511875000003</v>
       </c>
-      <c r="E12" s="51">
+      <c r="E12" s="47">
         <f t="shared" ref="E12:O12" si="0">E5*E6*E7*E8*E9*E10*E11</f>
         <v>1.1329619753086422</v>
       </c>
-      <c r="F12" s="51">
+      <c r="F12" s="47">
         <f t="shared" si="0"/>
         <v>1.1380050000000002</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="47">
         <f t="shared" si="0"/>
         <v>1.3276725</v>
       </c>
-      <c r="H12" s="51">
+      <c r="H12" s="47">
         <f t="shared" si="0"/>
         <v>1.0862775000000002</v>
       </c>
-      <c r="I12" s="51">
+      <c r="I12" s="47">
         <f t="shared" si="0"/>
         <v>1.2673237500000001</v>
       </c>
-      <c r="J12" s="51">
+      <c r="J12" s="47">
         <f t="shared" si="0"/>
         <v>1.2528592592592596</v>
       </c>
-      <c r="K12" s="51">
+      <c r="K12" s="47">
         <f t="shared" si="0"/>
         <v>1.2137074074074077</v>
       </c>
-      <c r="L12" s="51">
+      <c r="L12" s="47">
         <f t="shared" si="0"/>
         <v>1.2673237500000001</v>
       </c>
-      <c r="M12" s="51">
+      <c r="M12" s="47">
         <f t="shared" si="0"/>
         <v>1.5663913086419756</v>
       </c>
-      <c r="N12" s="51">
+      <c r="N12" s="47">
         <f t="shared" si="0"/>
         <v>1.2829278814814817</v>
       </c>
-      <c r="O12" s="51">
+      <c r="O12" s="47">
         <f t="shared" si="0"/>
         <v>1.2673237499999999</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="32" x14ac:dyDescent="0.2">
-      <c r="B13" s="49"/>
-      <c r="C13" s="52" t="s">
+      <c r="B13" s="45"/>
+      <c r="C13" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="53">
+      <c r="D13" s="49">
         <v>1.2033511875000003</v>
       </c>
-      <c r="E13" s="53">
+      <c r="E13" s="49">
         <v>1.1329619753086422</v>
       </c>
-      <c r="F13" s="53">
+      <c r="F13" s="49">
         <v>1.1380050000000002</v>
       </c>
-      <c r="G13" s="53">
+      <c r="G13" s="49">
         <v>1.25</v>
       </c>
-      <c r="H13" s="53">
+      <c r="H13" s="49">
         <v>1.0862775000000002</v>
       </c>
-      <c r="I13" s="53">
+      <c r="I13" s="49">
         <v>1.25</v>
       </c>
-      <c r="J13" s="53">
+      <c r="J13" s="49">
         <v>1.25</v>
       </c>
-      <c r="K13" s="53">
+      <c r="K13" s="49">
         <v>1.2137074074074077</v>
       </c>
-      <c r="L13" s="53">
+      <c r="L13" s="49">
         <v>1.25</v>
       </c>
-      <c r="M13" s="53">
+      <c r="M13" s="49">
         <v>1.25</v>
       </c>
-      <c r="N13" s="53">
+      <c r="N13" s="49">
         <v>1.25</v>
       </c>
-      <c r="O13" s="53">
+      <c r="O13" s="49">
         <v>1.25</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="55"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2974,18 +2974,18 @@
     <row r="3" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="39" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="40" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="29">
@@ -2999,7 +2999,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="41" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="30">
@@ -3013,13 +3013,13 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="33">
         <v>0.6</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="34">
         <v>0.8</v>
       </c>
       <c r="E7" s="26">
@@ -3027,7 +3027,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="41" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="30">
@@ -3041,7 +3041,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="41" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="30">
@@ -3055,7 +3055,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="41" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="30">
@@ -3069,13 +3069,13 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="35">
         <v>0.6</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="36">
         <v>0.8</v>
       </c>
       <c r="E11" s="27">
@@ -3096,8 +3096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C3:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3139,7 +3139,7 @@
         <v>24.930378023996418</v>
       </c>
       <c r="G5" s="20">
-        <v>30000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.2">
@@ -3156,7 +3156,7 @@
         <v>127.10047039378478</v>
       </c>
       <c r="G6" s="20">
-        <v>144000</v>
+        <v>78000</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.2">
@@ -3173,7 +3173,7 @@
         <v>94.902922219146646</v>
       </c>
       <c r="G7" s="20">
-        <v>108000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.2">
@@ -3190,7 +3190,7 @@
         <v>180.76747089361268</v>
       </c>
       <c r="G8" s="20">
-        <v>240000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.2">
@@ -3207,7 +3207,7 @@
         <v>77.328306993378746</v>
       </c>
       <c r="G9" s="20">
-        <v>84000</v>
+        <v>54000</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.2">
@@ -3224,7 +3224,7 @@
         <v>208.31299026787747</v>
       </c>
       <c r="G10" s="20">
-        <v>264000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.2">
@@ -3241,7 +3241,7 @@
         <v>201.13991107747606</v>
       </c>
       <c r="G11" s="20">
-        <v>252000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.2">
@@ -3258,7 +3258,7 @@
         <v>79.096493449821622</v>
       </c>
       <c r="G12" s="20">
-        <v>96000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.2">
@@ -3275,7 +3275,7 @@
         <v>61.547019851872889</v>
       </c>
       <c r="G13" s="20">
-        <v>78000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.2">
@@ -3292,7 +3292,7 @@
         <v>229.82762864798548</v>
       </c>
       <c r="G14" s="20">
-        <v>360000</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.2">
@@ -3309,7 +3309,7 @@
         <v>224.48650789896882</v>
       </c>
       <c r="G15" s="20">
-        <v>288000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="16" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3326,7 +3326,7 @@
         <v>67.859534708475252</v>
       </c>
       <c r="G16" s="22">
-        <v>86000</v>
+        <v>43200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>